<commit_message>
make some code more eficient
</commit_message>
<xml_diff>
--- a/hasil/2024-07-01_monitoring_lama_perkara.xlsx
+++ b/hasil/2024-07-01_monitoring_lama_perkara.xlsx
@@ -763,7 +763,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="10">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>13</v>
@@ -786,7 +786,7 @@
         <v>20</v>
       </c>
       <c r="F9" s="10">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>13</v>
@@ -809,7 +809,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="10">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>13</v>
@@ -832,7 +832,7 @@
         <v>23</v>
       </c>
       <c r="F11" s="10">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>13</v>
@@ -878,7 +878,7 @@
         <v>27</v>
       </c>
       <c r="F13" s="10">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>13</v>
@@ -947,7 +947,7 @@
         <v>20</v>
       </c>
       <c r="F16" s="10">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>13</v>
@@ -993,7 +993,7 @@
         <v>20</v>
       </c>
       <c r="F18" s="10">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>13</v>
@@ -1016,7 +1016,7 @@
         <v>20</v>
       </c>
       <c r="F19" s="10">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>13</v>
@@ -1062,7 +1062,7 @@
         <v>43</v>
       </c>
       <c r="F21" s="10">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>13</v>
@@ -1085,7 +1085,7 @@
         <v>46</v>
       </c>
       <c r="F22" s="10">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>13</v>
@@ -1108,7 +1108,7 @@
         <v>27</v>
       </c>
       <c r="F23" s="10">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>13</v>

</xml_diff>